<commit_message>
Overview: Completed user profile generation functionality.
FIX: Logic in KL Divergence dip detection method so that it works correctly for a low number of topics.
ADD: Methods to support time factor calculations and processing.
ADD: Methods to support log file loading and processing into an LDA model.
ADD: A routine for generating a user profile.
MOD: Updated the log maker's output format to be more suitable for string processing.
</commit_message>
<xml_diff>
--- a/formats/Equation.xlsx
+++ b/formats/Equation.xlsx
@@ -507,155 +507,155 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:U9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,14 +1347,14 @@
         <v>0.5</v>
       </c>
       <c r="N7" s="18"/>
-      <c r="P7" s="34" t="s">
+      <c r="P7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="36"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="22"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1401,12 +1401,12 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="N8" s="18"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="39"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="25"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1453,12 +1453,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="42"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="28"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1551,14 +1551,14 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="N11" s="18"/>
-      <c r="P11" s="43" t="s">
+      <c r="P11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="44"/>
-      <c r="U11" s="45"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="31"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1605,12 +1605,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="N12" s="18"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="47"/>
-      <c r="U12" s="48"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="34"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1657,12 +1657,12 @@
         <v>0</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="51"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="37"/>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1709,14 +1709,14 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="N14" s="18"/>
-      <c r="P14" s="52" t="s">
+      <c r="P14" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="Q14" s="53"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="54"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="40"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1763,12 +1763,12 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="N15" s="18"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="57"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="43"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1861,14 +1861,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="N17" s="18"/>
-      <c r="P17" s="58" t="s">
+      <c r="P17" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="59"/>
-      <c r="S17" s="59"/>
-      <c r="T17" s="59"/>
-      <c r="U17" s="60"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="46"/>
     </row>
     <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1915,14 +1915,14 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="P18" s="61" t="s">
+      <c r="P18" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="Q18" s="62"/>
-      <c r="R18" s="62"/>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="63"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="49"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1969,12 +1969,12 @@
         <v>0.5</v>
       </c>
       <c r="N19" s="18"/>
-      <c r="P19" s="64"/>
-      <c r="Q19" s="65"/>
-      <c r="R19" s="65"/>
-      <c r="S19" s="65"/>
-      <c r="T19" s="65"/>
-      <c r="U19" s="66"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="52"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -2021,12 +2021,12 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N20" s="18"/>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="68"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="68"/>
-      <c r="T20" s="68"/>
-      <c r="U20" s="69"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
+      <c r="T20" s="54"/>
+      <c r="U20" s="55"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -2082,11 +2082,11 @@
       <c r="R21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S21" s="20" t="s">
+      <c r="S21" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="T21" s="20"/>
-      <c r="U21" s="26"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="60"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -2142,12 +2142,12 @@
       <c r="R22" s="7">
         <v>30</v>
       </c>
-      <c r="S22" s="21">
+      <c r="S22" s="61">
         <f>ABS(((Q22*60+R22)-720)/720)</f>
         <v>0.95833333333333337</v>
       </c>
-      <c r="T22" s="21"/>
-      <c r="U22" s="27"/>
+      <c r="T22" s="61"/>
+      <c r="U22" s="62"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2203,12 +2203,12 @@
       <c r="R23" s="10">
         <v>45</v>
       </c>
-      <c r="S23" s="28">
+      <c r="S23" s="63">
         <f>ABS(((Q23*60+R23)-720)/720)</f>
         <v>0.60416666666666663</v>
       </c>
-      <c r="T23" s="28"/>
-      <c r="U23" s="29"/>
+      <c r="T23" s="63"/>
+      <c r="U23" s="64"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2255,14 +2255,14 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="P24" s="23" t="s">
+      <c r="P24" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="25"/>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="57"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="58"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2309,17 +2309,17 @@
         <v>1</v>
       </c>
       <c r="N25" s="18"/>
-      <c r="P25" s="30" t="s">
+      <c r="P25" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
-      <c r="S25" s="32">
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
+      <c r="S25" s="67">
         <f>ABS(((1*60+0)-720)/720)</f>
         <v>0.91666666666666663</v>
       </c>
-      <c r="T25" s="32"/>
-      <c r="U25" s="33"/>
+      <c r="T25" s="67"/>
+      <c r="U25" s="68"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="5"/>
@@ -2333,14 +2333,14 @@
       <c r="P26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="20" t="s">
+      <c r="Q26" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20" t="s">
+      <c r="R26" s="59"/>
+      <c r="S26" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="T26" s="20"/>
+      <c r="T26" s="59"/>
       <c r="U26" s="13" t="s">
         <v>26</v>
       </c>
@@ -2363,16 +2363,16 @@
       <c r="P27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="61">
         <f>S22</f>
         <v>0.95833333333333337</v>
       </c>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21">
+      <c r="R27" s="61"/>
+      <c r="S27" s="61">
         <f>1-ABS(Q27-$S$25)</f>
         <v>0.95833333333333326</v>
       </c>
-      <c r="T27" s="21"/>
+      <c r="T27" s="61"/>
       <c r="U27" s="14" t="s">
         <v>27</v>
       </c>
@@ -2381,37 +2381,37 @@
       <c r="P28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Q28" s="22">
+      <c r="Q28" s="69">
         <f>S23</f>
         <v>0.60416666666666663</v>
       </c>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22">
+      <c r="R28" s="69"/>
+      <c r="S28" s="69">
         <f>1-ABS(Q28-$S$25)</f>
         <v>0.6875</v>
       </c>
-      <c r="T28" s="22"/>
+      <c r="T28" s="69"/>
       <c r="U28" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="P7:U9"/>
-    <mergeCell ref="P11:U13"/>
-    <mergeCell ref="P14:U15"/>
-    <mergeCell ref="P17:U17"/>
-    <mergeCell ref="P18:U20"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
     <mergeCell ref="P24:U24"/>
     <mergeCell ref="S21:U21"/>
     <mergeCell ref="S22:U22"/>
     <mergeCell ref="S23:U23"/>
     <mergeCell ref="P25:R25"/>
     <mergeCell ref="S25:U25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="P7:U9"/>
+    <mergeCell ref="P11:U13"/>
+    <mergeCell ref="P14:U15"/>
+    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="P18:U20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Overview: Completed feasibility demo preparation.
FIX: Updated topic factor equation and weighting formula to solve the looping/abiguity issue.
ADD: Mechanisms for determing most relevant topic based on time.
MOD: Added i/o for testing time relevance.
MOD: Updated the code to be demo ready.
</commit_message>
<xml_diff>
--- a/formats/Equation.xlsx
+++ b/formats/Equation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Hour</t>
   </si>
@@ -81,15 +81,9 @@
     <t>Minutes</t>
   </si>
   <si>
-    <t>The user profile contains two topics. Topic T1 is more relevant at 23:30 and Topic T2 is more relevant at 04:45. For topic modeling calculate the time factors which will appear in the user profile:</t>
-  </si>
-  <si>
     <t>Find which topic is more relevant at 01:00, for use in re-ranking:</t>
   </si>
   <si>
-    <t>Weighting = 1 - abs(Topic_TimeFactor - CurrentTime_TimeFactor) … (2)</t>
-  </si>
-  <si>
     <t>Weighting using (2)</t>
   </si>
   <si>
@@ -105,7 +99,16 @@
     <t>Current Time - Time Factor for 01:00 using (1):</t>
   </si>
   <si>
-    <t>TimeFactor = abs(((Hours*60+Minutes)-720)/720) … (1)</t>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>TimeFactor = abs((Hours*60+Minutes)/1440) … (1)</t>
+  </si>
+  <si>
+    <t>Weighting = 1 - (abs(Topic_TimeFactor - CurrentTime_TimeFactor), 1 - abs(Topic_TimeFactor - CurrentTime_TimeFactor)) … (2)</t>
+  </si>
+  <si>
+    <t>The user profile contains three topics. Topic T1 is more relevant at 23:55, Topic T2 is more relevant at 04:45 and Topic T3 is more relevant at 23:00. For topic modeling calculate the time factors which will appear in the user profile:</t>
   </si>
 </sst>
 </file>
@@ -502,11 +505,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,25 +642,22 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -958,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17:U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +988,7 @@
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" customWidth="1"/>
     <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="21" max="21" width="85.42578125" customWidth="1"/>
     <col min="23" max="23" width="19.85546875" customWidth="1"/>
     <col min="24" max="24" width="3.5703125" customWidth="1"/>
   </cols>
@@ -1034,7 +1037,7 @@
       <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="19"/>
+      <c r="R1" s="18"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1090,7 +1093,7 @@
         <f>ABS(((O2*60+P2)-720)/720)</f>
         <v>0.29166666666666669</v>
       </c>
-      <c r="R2" s="18"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1147,7 +1150,7 @@
         <f>ABS(((O3*60+P3)-720)/720)</f>
         <v>0.39583333333333331</v>
       </c>
-      <c r="R3" s="18"/>
+      <c r="R3" s="17"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1204,7 +1207,7 @@
         <f>ABS(((O4*60+P4)-720)/720)</f>
         <v>1</v>
       </c>
-      <c r="R4" s="18"/>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1250,11 +1253,11 @@
         <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="17"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -1300,7 +1303,7 @@
         <f t="shared" si="5"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="N6" s="18"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1346,15 +1349,15 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="P7" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="22"/>
+      <c r="N7" s="17"/>
+      <c r="P7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="23"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1400,13 +1403,13 @@
         <f t="shared" si="5"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="N8" s="18"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="25"/>
+      <c r="N8" s="17"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="26"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1452,13 +1455,13 @@
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="28"/>
+      <c r="N9" s="17"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="29"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1504,7 +1507,7 @@
         <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
-      <c r="N10" s="18"/>
+      <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1550,15 +1553,15 @@
         <f t="shared" si="5"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="N11" s="18"/>
-      <c r="P11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="31"/>
+      <c r="N11" s="17"/>
+      <c r="P11" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="32"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1604,13 +1607,13 @@
         <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="N12" s="18"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="33"/>
-      <c r="T12" s="33"/>
-      <c r="U12" s="34"/>
+      <c r="N12" s="17"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="35"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1656,13 +1659,13 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N13" s="18"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="37"/>
+      <c r="N13" s="17"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="38"/>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1708,15 +1711,15 @@
         <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="N14" s="18"/>
-      <c r="P14" s="38" t="s">
+      <c r="N14" s="17"/>
+      <c r="P14" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="41"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1762,13 +1765,13 @@
         <f t="shared" si="5"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="43"/>
+      <c r="N15" s="17"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="44"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1814,7 +1817,7 @@
         <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
-      <c r="N16" s="18"/>
+      <c r="N16" s="17"/>
     </row>
     <row r="17" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1860,15 +1863,15 @@
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N17" s="18"/>
-      <c r="P17" s="44" t="s">
+      <c r="N17" s="17"/>
+      <c r="P17" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="47"/>
     </row>
     <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1914,15 +1917,15 @@
         <f t="shared" si="5"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="P18" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="49"/>
+      <c r="N18" s="17"/>
+      <c r="P18" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="50"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1968,13 +1971,13 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="N19" s="18"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="52"/>
+      <c r="N19" s="17"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="53"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -2020,13 +2023,13 @@
         <f t="shared" si="5"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="N20" s="18"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="54"/>
-      <c r="T20" s="54"/>
-      <c r="U20" s="55"/>
+      <c r="N20" s="17"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="55"/>
+      <c r="U20" s="56"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -2072,7 +2075,7 @@
         <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="N21" s="18"/>
+      <c r="N21" s="17"/>
       <c r="P21" s="11" t="s">
         <v>16</v>
       </c>
@@ -2082,11 +2085,11 @@
       <c r="R21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S21" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="T21" s="59"/>
-      <c r="U21" s="60"/>
+      <c r="S21" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="T21" s="60"/>
+      <c r="U21" s="61"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -2132,7 +2135,7 @@
         <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
-      <c r="N22" s="18"/>
+      <c r="N22" s="17"/>
       <c r="P22" s="6" t="s">
         <v>17</v>
       </c>
@@ -2140,14 +2143,14 @@
         <v>23</v>
       </c>
       <c r="R22" s="7">
-        <v>30</v>
-      </c>
-      <c r="S22" s="61">
-        <f>ABS(((Q22*60+R22)-720)/720)</f>
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="T22" s="61"/>
-      <c r="U22" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="S22" s="62">
+        <f>ABS((Q22*60+R22)/1440)</f>
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="T22" s="62"/>
+      <c r="U22" s="63"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2193,24 +2196,24 @@
         <f t="shared" si="5"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="N23" s="18"/>
-      <c r="P23" s="12" t="s">
+      <c r="N23" s="17"/>
+      <c r="P23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="Q23" s="7">
         <v>4</v>
       </c>
-      <c r="R23" s="10">
+      <c r="R23" s="7">
         <v>45</v>
       </c>
-      <c r="S23" s="63">
-        <f>ABS(((Q23*60+R23)-720)/720)</f>
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="T23" s="63"/>
-      <c r="U23" s="64"/>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S23" s="62">
+        <f t="shared" ref="S23:S24" si="7">ABS((Q23*60+R23)/1440)</f>
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="T23" s="62"/>
+      <c r="U23" s="63"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>A23+1</f>
         <v>22</v>
@@ -2254,17 +2257,24 @@
         <f t="shared" si="5"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="N24" s="18"/>
-      <c r="P24" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q24" s="57"/>
-      <c r="R24" s="57"/>
-      <c r="S24" s="57"/>
-      <c r="T24" s="57"/>
-      <c r="U24" s="58"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N24" s="17"/>
+      <c r="P24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="10">
+        <v>23</v>
+      </c>
+      <c r="R24" s="10">
+        <v>0</v>
+      </c>
+      <c r="S24" s="68">
+        <f t="shared" si="7"/>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="T24" s="68"/>
+      <c r="U24" s="69"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="6"/>
         <v>23</v>
@@ -2308,18 +2318,15 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="N25" s="18"/>
-      <c r="P25" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q25" s="66"/>
-      <c r="R25" s="66"/>
-      <c r="S25" s="67">
-        <f>ABS(((1*60+0)-720)/720)</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="T25" s="67"/>
-      <c r="U25" s="68"/>
+      <c r="N25" s="17"/>
+      <c r="P25" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="59"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="5"/>
@@ -2329,89 +2336,121 @@
       <c r="K26" s="5"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="18"/>
-      <c r="P26" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q26" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="T26" s="59"/>
-      <c r="U26" s="13" t="s">
+      <c r="N26" s="17"/>
+      <c r="P26" s="64" t="s">
         <v>26</v>
       </c>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="65"/>
+      <c r="S26" s="66">
+        <f>ABS((1*60+0)/1440)</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T26" s="66"/>
+      <c r="U26" s="67"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
-      <c r="P27" s="6" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="16"/>
+      <c r="P27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="R27" s="60"/>
+      <c r="S27" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="T27" s="60"/>
+      <c r="U27" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="61">
+      <c r="Q28" s="62">
         <f>S22</f>
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="R28" s="62"/>
+      <c r="S28" s="62">
+        <f>1-MIN(ABS(Q28-$S$26), 1-ABS(Q28-$S$26))</f>
+        <v>0.95486111111111116</v>
+      </c>
+      <c r="T28" s="62"/>
+      <c r="U28" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q29" s="62">
+        <f>S23</f>
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="R29" s="62"/>
+      <c r="S29" s="62">
+        <f t="shared" ref="S29:S30" si="8">1-MIN(ABS(Q29-$S$26), 1-ABS(Q29-$S$26))</f>
+        <v>0.84375</v>
+      </c>
+      <c r="T29" s="62"/>
+      <c r="U29" s="14"/>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="20">
+        <f>S24</f>
         <v>0.95833333333333337</v>
       </c>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61">
-        <f>1-ABS(Q27-$S$25)</f>
-        <v>0.95833333333333326</v>
-      </c>
-      <c r="T27" s="61"/>
-      <c r="U27" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q28" s="69">
-        <f>S23</f>
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="R28" s="69"/>
-      <c r="S28" s="69">
-        <f>1-ABS(Q28-$S$25)</f>
-        <v>0.6875</v>
-      </c>
-      <c r="T28" s="69"/>
-      <c r="U28" s="15"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="20">
+        <f t="shared" si="8"/>
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="T30" s="20"/>
+      <c r="U30" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="S26:T26"/>
+  <mergeCells count="20">
+    <mergeCell ref="Q29:R29"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="S28:T28"/>
-    <mergeCell ref="P24:U24"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="S30:T30"/>
     <mergeCell ref="P7:U9"/>
     <mergeCell ref="P11:U13"/>
     <mergeCell ref="P14:U15"/>
     <mergeCell ref="P17:U17"/>
     <mergeCell ref="P18:U20"/>
+    <mergeCell ref="P25:U25"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Overview: Preperation for total project integration.
Mod: Refactored the chrome interface to use our naming scheme.
Mod: Updated formats to suit what was discussed in meetings.
Mod: Updated modeller to include a benchmark mode for use in evaluation.
Mod: Multi-threaded modeller model building process to improve performace.
Mod: Various bug fixes and updates.
</commit_message>
<xml_diff>
--- a/formats/Equation.xlsx
+++ b/formats/Equation.xlsx
@@ -105,10 +105,10 @@
     <t>TimeFactor = abs((Hours*60+Minutes)/1440) … (1)</t>
   </si>
   <si>
-    <t>Weighting = 1 - (abs(Topic_TimeFactor - CurrentTime_TimeFactor), 1 - abs(Topic_TimeFactor - CurrentTime_TimeFactor)) … (2)</t>
-  </si>
-  <si>
     <t>The user profile contains three topics. Topic T1 is more relevant at 23:55, Topic T2 is more relevant at 04:45 and Topic T3 is more relevant at 23:00. For topic modeling calculate the time factors which will appear in the user profile:</t>
+  </si>
+  <si>
+    <t>Weighting = 1 - min(abs(Topic_TimeFactor - CurrentTime_TimeFactor), 1 - abs(Topic_TimeFactor - CurrentTime_TimeFactor)) … (2)</t>
   </si>
 </sst>
 </file>
@@ -510,6 +510,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,13 +636,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -964,7 +964,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:U30"/>
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,14 +1350,14 @@
         <v>0.5</v>
       </c>
       <c r="N7" s="17"/>
-      <c r="P7" s="21" t="s">
+      <c r="P7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="23"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="25"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1404,12 +1404,12 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="N8" s="17"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="28"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1456,12 +1456,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="N9" s="17"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1554,14 +1554,14 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="N11" s="17"/>
-      <c r="P11" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="32"/>
+      <c r="P11" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="34"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1608,12 +1608,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="N12" s="17"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="37"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1660,12 +1660,12 @@
         <v>0</v>
       </c>
       <c r="N13" s="17"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="40"/>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1712,14 +1712,14 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="N14" s="17"/>
-      <c r="P14" s="39" t="s">
+      <c r="P14" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="40"/>
-      <c r="T14" s="40"/>
-      <c r="U14" s="41"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="43"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1766,12 +1766,12 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="N15" s="17"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="43"/>
-      <c r="T15" s="43"/>
-      <c r="U15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="46"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1864,14 +1864,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="N17" s="17"/>
-      <c r="P17" s="45" t="s">
+      <c r="P17" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="47"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="49"/>
     </row>
     <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1918,14 +1918,14 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="N18" s="17"/>
-      <c r="P18" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="50"/>
+      <c r="P18" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="52"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1972,12 +1972,12 @@
         <v>0.5</v>
       </c>
       <c r="N19" s="17"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="52"/>
-      <c r="R19" s="52"/>
-      <c r="S19" s="52"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="54"/>
+      <c r="U19" s="55"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -2024,12 +2024,12 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N20" s="17"/>
-      <c r="P20" s="54"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="55"/>
-      <c r="S20" s="55"/>
-      <c r="T20" s="55"/>
-      <c r="U20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="58"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -2085,11 +2085,11 @@
       <c r="R21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S21" s="60" t="s">
+      <c r="S21" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="T21" s="60"/>
-      <c r="U21" s="61"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="62"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -2145,11 +2145,11 @@
       <c r="R22" s="7">
         <v>55</v>
       </c>
-      <c r="S22" s="62">
+      <c r="S22" s="20">
         <f>ABS((Q22*60+R22)/1440)</f>
         <v>0.99652777777777779</v>
       </c>
-      <c r="T22" s="62"/>
+      <c r="T22" s="20"/>
       <c r="U22" s="63"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -2206,11 +2206,11 @@
       <c r="R23" s="7">
         <v>45</v>
       </c>
-      <c r="S23" s="62">
+      <c r="S23" s="20">
         <f t="shared" ref="S23:S24" si="7">ABS((Q23*60+R23)/1440)</f>
         <v>0.19791666666666666</v>
       </c>
-      <c r="T23" s="62"/>
+      <c r="T23" s="20"/>
       <c r="U23" s="63"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2319,14 +2319,14 @@
         <v>1</v>
       </c>
       <c r="N25" s="17"/>
-      <c r="P25" s="57" t="s">
+      <c r="P25" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="59"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="61"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="5"/>
@@ -2367,14 +2367,14 @@
       <c r="P27" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="60" t="s">
+      <c r="Q27" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="R27" s="60"/>
-      <c r="S27" s="60" t="s">
+      <c r="R27" s="21"/>
+      <c r="S27" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="60"/>
+      <c r="T27" s="21"/>
       <c r="U27" s="13" t="s">
         <v>24</v>
       </c>
@@ -2383,16 +2383,16 @@
       <c r="P28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="62">
+      <c r="Q28" s="20">
         <f>S22</f>
         <v>0.99652777777777779</v>
       </c>
-      <c r="R28" s="62"/>
-      <c r="S28" s="62">
+      <c r="R28" s="20"/>
+      <c r="S28" s="20">
         <f>1-MIN(ABS(Q28-$S$26), 1-ABS(Q28-$S$26))</f>
         <v>0.95486111111111116</v>
       </c>
-      <c r="T28" s="62"/>
+      <c r="T28" s="20"/>
       <c r="U28" s="14" t="s">
         <v>25</v>
       </c>
@@ -2401,47 +2401,36 @@
       <c r="P29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q29" s="62">
+      <c r="Q29" s="20">
         <f>S23</f>
         <v>0.19791666666666666</v>
       </c>
-      <c r="R29" s="62"/>
-      <c r="S29" s="62">
+      <c r="R29" s="20"/>
+      <c r="S29" s="20">
         <f t="shared" ref="S29:S30" si="8">1-MIN(ABS(Q29-$S$26), 1-ABS(Q29-$S$26))</f>
         <v>0.84375</v>
       </c>
-      <c r="T29" s="62"/>
+      <c r="T29" s="20"/>
       <c r="U29" s="14"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P30" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q30" s="20">
+      <c r="Q30" s="22">
         <f>S24</f>
         <v>0.95833333333333337</v>
       </c>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20">
+      <c r="R30" s="22"/>
+      <c r="S30" s="22">
         <f t="shared" si="8"/>
         <v>0.91666666666666674</v>
       </c>
-      <c r="T30" s="20"/>
+      <c r="T30" s="22"/>
       <c r="U30" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="P7:U9"/>
-    <mergeCell ref="P11:U13"/>
-    <mergeCell ref="P14:U15"/>
-    <mergeCell ref="P17:U17"/>
-    <mergeCell ref="P18:U20"/>
     <mergeCell ref="P25:U25"/>
     <mergeCell ref="S21:U21"/>
     <mergeCell ref="S22:U22"/>
@@ -2449,6 +2438,17 @@
     <mergeCell ref="P26:R26"/>
     <mergeCell ref="S26:U26"/>
     <mergeCell ref="S24:U24"/>
+    <mergeCell ref="P7:U9"/>
+    <mergeCell ref="P11:U13"/>
+    <mergeCell ref="P14:U15"/>
+    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="P18:U20"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="S30:T30"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q28:R28"/>
   </mergeCells>

</xml_diff>